<commit_message>
Inclusão de novos casos de teste
Incluído: Manter Sprint;
Alterados: Manter Empresa e Manter Usuário.
</commit_message>
<xml_diff>
--- a/trunk/doc/testes/CT - Manter Empresa.xlsx
+++ b/trunk/doc/testes/CT - Manter Empresa.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
   <si>
     <t>Scrumming</t>
   </si>
@@ -111,6 +111,21 @@
   </si>
   <si>
     <t>O cadastro de empresa deverá ser cancelado e o sistema deverá retornar para a tela de login.</t>
+  </si>
+  <si>
+    <t>Efetuar sem sucesso o cadastro/alteração de uma empresa. Empresa já cadastrada.
+Ter executado com sucesso o passo #2.</t>
+  </si>
+  <si>
+    <t>1- Acessar o link para efetuar o registro.
+2- Preencher os campos "Nome da Empresa" com um nome igual a de uma empresa já cadastrada.</t>
+  </si>
+  <si>
+    <t>Empresa não deverá ser cadastrada.
+Deverá ser exibida a mensagem de que a empresa já existe.</t>
+  </si>
+  <si>
+    <t>02.00 - 18/04/2014</t>
   </si>
 </sst>
 </file>
@@ -192,7 +207,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -214,6 +229,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -512,9 +530,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
@@ -527,7 +543,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="2:2">
+    <row r="5" spans="2:2" ht="18">
       <c r="B5" s="2" t="s">
         <v>8</v>
       </c>
@@ -544,9 +560,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
@@ -571,8 +585,12 @@
       </c>
     </row>
     <row r="3" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
+      <c r="A3" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>3</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -677,11 +695,17 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="12.75">
+    <row r="7" spans="1:4" ht="51">
       <c r="A7" s="4"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
+      <c r="B7" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="8" spans="1:4" ht="12.75">
       <c r="A8" s="4"/>

</xml_diff>